<commit_message>
Update to Accomplishment Log
New Columns
</commit_message>
<xml_diff>
--- a/Accomplishment Log/AccomplishmentLogV1.0.xlsx
+++ b/Accomplishment Log/AccomplishmentLogV1.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Q3 2017</t>
+  </si>
+  <si>
+    <t>Problem Solved</t>
+  </si>
+  <si>
+    <t>Opportunity Created</t>
   </si>
 </sst>
 </file>
@@ -73,7 +79,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -104,9 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -114,9 +120,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -128,7 +131,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="13">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -154,10 +166,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -174,17 +186,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FA1D97-7DC8-8D41-94DA-C1180D7DE639}" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0" dataDxfId="7">
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{57904901-37E9-174A-A377-3F072C8781FF}" name="Date" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{2551C189-12DB-B144-A775-C86FEE61EE29}" name="Accomplishment" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{88DCC13B-722F-D54E-9B1B-2FC208C91C65}" name="Project" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{D3D008ED-2BE6-144E-A5C8-E3FE200B9510}" name="Benefit" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{9CCBB3F9-0BA2-D040-A76F-40644FD708C7}" name="Person Impacted" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{B5F6C671-1148-0E4B-8A34-714FB235D85B}" name="Business Impact" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{68C31D0C-8E27-3541-B2BA-2CA24875ACFC}" name="Impact" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{EA3C54DB-DBB2-4940-8D04-7C04857EF827}" name="Dollar Impact" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{71E3F602-0C10-1344-A335-ECA9437E9630}" name="Mentioned In Review Period" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31FA1D97-7DC8-8D41-94DA-C1180D7DE639}" name="Table1" displayName="Table1" ref="A1:K2" totalsRowShown="0" headerRowDxfId="1" dataDxfId="12">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{57904901-37E9-174A-A377-3F072C8781FF}" name="Date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{2551C189-12DB-B144-A775-C86FEE61EE29}" name="Accomplishment" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{88DCC13B-722F-D54E-9B1B-2FC208C91C65}" name="Project" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D3D008ED-2BE6-144E-A5C8-E3FE200B9510}" name="Benefit" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{9CCBB3F9-0BA2-D040-A76F-40644FD708C7}" name="Person Impacted" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{B5F6C671-1148-0E4B-8A34-714FB235D85B}" name="Business Impact" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{68C31D0C-8E27-3541-B2BA-2CA24875ACFC}" name="Impact" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{EA3C54DB-DBB2-4940-8D04-7C04857EF827}" name="Dollar Impact" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{71E3F602-0C10-1344-A335-ECA9437E9630}" name="Mentioned In Review Period" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{B82A9798-CA7B-804B-B4B7-BD494B2FC23A}" name="Problem Solved" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{1D14A4E2-162B-1049-B644-523AA0154E06}" name="Opportunity Created" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -487,16 +501,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BA91EA-AE2E-A24A-A0DB-66E6CA0F3D29}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="36.6640625" customWidth="1"/>
@@ -505,11 +520,11 @@
     <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="32">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -530,11 +545,17 @@
       <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="48">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="48">
       <c r="A2" s="1">
         <v>42911</v>
       </c>
@@ -551,11 +572,13 @@
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>